<commit_message>
added pce data load
</commit_message>
<xml_diff>
--- a/InputData/BEA/pce1018.xlsx
+++ b/InputData/BEA/pce1018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataBootcamp\Projects\GTATL5Project2\BEA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\REGIONAL\newsrel\working\1018pce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1796DA17-62E9-49F1-8B8A-D8216F6A6F3B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0F7B2CDC-CDCF-4941-9886-40A7082FF7BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -5707,8 +5707,8 @@
   </sheetPr>
   <dimension ref="A1:Q117"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8280,7 +8280,7 @@
   <dimension ref="A1:Q117"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14538,8 +14538,8 @@
   </sheetPr>
   <dimension ref="A1:Q117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18429,7 +18429,7 @@
   <dimension ref="A1:Q117"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22187,7 +22187,7 @@
   <dimension ref="A1:Q117"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -24994,7 +24994,7 @@
   <dimension ref="A1:Q117"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>